<commit_message>
added final nets to gui and added results - over and out!
</commit_message>
<xml_diff>
--- a/Exercise 2/resultsOfPredefinedNetworks/results.xlsx
+++ b/Exercise 2/resultsOfPredefinedNetworks/results.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian Rhelfedt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian Rhelfedt\Desktop\Machine-Learning\Exercise 2\resultsOfPredefinedNetworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="preDefined" sheetId="1" r:id="rId1"/>
+    <sheet name="Final" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="150">
   <si>
     <t>Feed-forward with backprobagation</t>
   </si>
@@ -357,6 +358,123 @@
   </si>
   <si>
     <t>0.71</t>
+  </si>
+  <si>
+    <t>Recurrent</t>
+  </si>
+  <si>
+    <t>FF (high)</t>
+  </si>
+  <si>
+    <t>FF (medium)</t>
+  </si>
+  <si>
+    <t>0.527</t>
+  </si>
+  <si>
+    <t>0.907</t>
+  </si>
+  <si>
+    <t>0.9995</t>
+  </si>
+  <si>
+    <t>0.734</t>
+  </si>
+  <si>
+    <t>0.282</t>
+  </si>
+  <si>
+    <t>0.636</t>
+  </si>
+  <si>
+    <t>0.344</t>
+  </si>
+  <si>
+    <t>0.677</t>
+  </si>
+  <si>
+    <t>0.682</t>
+  </si>
+  <si>
+    <t>0.887</t>
+  </si>
+  <si>
+    <t>0.9997</t>
+  </si>
+  <si>
+    <t>0.706</t>
+  </si>
+  <si>
+    <t>0.856</t>
+  </si>
+  <si>
+    <t>Detection (FF high)</t>
+  </si>
+  <si>
+    <t>Prediction (FF medium)</t>
+  </si>
+  <si>
+    <t>0.329</t>
+  </si>
+  <si>
+    <t>0.069</t>
+  </si>
+  <si>
+    <t>0.184</t>
+  </si>
+  <si>
+    <t>0.126</t>
+  </si>
+  <si>
+    <t>0.104</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>0.9993</t>
+  </si>
+  <si>
+    <t>0.609</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>0.023</t>
+  </si>
+  <si>
+    <t>0.455</t>
+  </si>
+  <si>
+    <t>0.761</t>
+  </si>
+  <si>
+    <t>0.008</t>
+  </si>
+  <si>
+    <t>0.397</t>
+  </si>
+  <si>
+    <t>0.853</t>
+  </si>
+  <si>
+    <t>0.0123</t>
+  </si>
+  <si>
+    <t>0.355</t>
+  </si>
+  <si>
+    <t>0.896</t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>0.473</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -460,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,6 +615,19 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,9 +922,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:20" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
       <c r="K1" t="s">
         <v>0</v>
       </c>
@@ -801,25 +932,15 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="G2" s="15"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
     <row r="3" spans="3:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="13"/>
       <c r="K3" s="3"/>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -836,14 +957,9 @@
       </c>
     </row>
     <row r="4" spans="3:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="13"/>
       <c r="K4" s="3" t="s">
         <v>2</v>
       </c>
@@ -864,14 +980,9 @@
       </c>
     </row>
     <row r="5" spans="3:20" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="13"/>
       <c r="K5" s="4" t="s">
         <v>3</v>
       </c>
@@ -892,14 +1003,9 @@
       </c>
     </row>
     <row r="6" spans="3:20" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="13"/>
       <c r="K6" s="3" t="s">
         <v>4</v>
       </c>
@@ -920,14 +1026,13 @@
       </c>
     </row>
     <row r="7" spans="3:20" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="13"/>
       <c r="K7" s="5" t="s">
         <v>5</v>
       </c>
@@ -947,12 +1052,44 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
       <c r="K9" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
       <c r="K11" s="3"/>
       <c r="L11" s="1" t="s">
         <v>1</v>
@@ -968,6 +1105,13 @@
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
       <c r="K12" s="3" t="s">
         <v>2</v>
       </c>
@@ -985,6 +1129,13 @@
       </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
       <c r="K13" s="4" t="s">
         <v>3</v>
       </c>
@@ -1002,6 +1153,13 @@
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
       <c r="K14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1780,4 +1938,359 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="F10" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>